<commit_message>
Multi-aggregated results and additional plots
</commit_message>
<xml_diff>
--- a/Conceptual_model.xlsx
+++ b/Conceptual_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\COVID2030\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\COVID-30\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143B0C39-7771-439E-97F9-7CC922DEAB82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6728481-CCCB-42BB-B435-B6A80AC89B5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4A8EDEA0-47F7-490C-BAE2-09782BA57031}"/>
+    <workbookView xWindow="-38520" yWindow="-5445" windowWidth="38640" windowHeight="21240" xr2:uid="{4A8EDEA0-47F7-490C-BAE2-09782BA57031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$X$51:$X$60</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$E$82:$N$86</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$P$82</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$E$82:$N$86</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
@@ -36,7 +36,7 @@
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!$E$89:$N$93</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!$E$89</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!$E$89:$N$93</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="47">
   <si>
     <t>Legenda</t>
   </si>
@@ -212,15 +212,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0;\-;\-"/>
     <numFmt numFmtId="165" formatCode="0;\-0;\-"/>
     <numFmt numFmtId="166" formatCode="0;0;\-"/>
     <numFmt numFmtId="167" formatCode="0.000;\-;\-"/>
     <numFmt numFmtId="168" formatCode="0.000;0.000;\-"/>
-    <numFmt numFmtId="169" formatCode="0.0;0.0;\-"/>
     <numFmt numFmtId="170" formatCode="0.0%"/>
     <numFmt numFmtId="171" formatCode="0.000"/>
-    <numFmt numFmtId="172" formatCode="0.00;0.00;\-"/>
+    <numFmt numFmtId="175" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -528,11 +528,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -607,14 +608,6 @@
     <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="10" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="10" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="170" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -661,15 +654,14 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="9" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="9" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -691,22 +683,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>3810</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>78105</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>3811</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="198" name="OpenSolver1">
+        <xdr:cNvPr id="194" name="OpenSolver1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CD84012-F3B4-443A-B4E0-5BE367A5381F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6543D17-30AC-4C15-9C3D-648D5217496A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -714,8 +706,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11795760" y="9212580"/>
-          <a:ext cx="609600" cy="1836420"/>
+          <a:off x="12938760" y="9212580"/>
+          <a:ext cx="609601" cy="1836420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -779,22 +771,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>3810</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>100965</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>3811</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>102870</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="199" name="OpenSolver2">
+        <xdr:cNvPr id="195" name="OpenSolver2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDC78590-A71B-4602-A6B1-089492452C44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64A27EC6-0363-45A1-B1A5-807EE04D82E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -802,8 +794,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11795760" y="11597640"/>
-          <a:ext cx="609600" cy="182880"/>
+          <a:off x="12938760" y="11597640"/>
+          <a:ext cx="609601" cy="182880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -860,23 +852,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>43629</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>50352</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1740535</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>18415</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>221146</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>173766</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>240980</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>145415</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="200" name="OpenSolver3">
+        <xdr:cNvPr id="196" name="OpenSolver3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AF90CA9-BE8C-4F76-8E0B-39E75B4F210A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{127868E2-F3DC-4478-83FC-02288695A9DB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -884,8 +876,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12997629" y="11256234"/>
-          <a:ext cx="1396717" cy="123414"/>
+          <a:off x="12922885" y="11515090"/>
+          <a:ext cx="253045" cy="127000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -954,22 +946,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>3811</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>78105</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>3811</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="201" name="OpenSolverX51:X60">
+        <xdr:cNvPr id="197" name="OpenSolverX51:X60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E1AFA37-E807-48F7-9AAF-CE67A402CB4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B292CF2F-24BE-4974-8018-B593BBCDECF2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -977,7 +969,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15453361" y="9212580"/>
+          <a:off x="16596361" y="9212580"/>
           <a:ext cx="609600" cy="1836420"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1039,22 +1031,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>5715</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>146686</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="202" name="OpenSolver5">
+        <xdr:cNvPr id="206" name="OpenSolver5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B04F22B-8591-414C-9707-32DF3AC62A79}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D060B73D-64A5-4DBE-9320-182059098A9F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1062,8 +1054,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3634740" y="14904720"/>
-          <a:ext cx="6332220" cy="914400"/>
+          <a:off x="3634740" y="16184880"/>
+          <a:ext cx="617220" cy="182881"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1120,23 +1112,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>131445</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="203" name="OpenSolver6">
+        <xdr:cNvPr id="207" name="OpenSolver6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD77D2C4-F98C-40A4-9B44-26311ED51677}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7964A4D-AD18-402F-BF26-84C2D4F780CE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1144,8 +1136,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3634740" y="16184880"/>
-          <a:ext cx="6332220" cy="914400"/>
+          <a:off x="10576560" y="14904720"/>
+          <a:ext cx="609600" cy="182880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1196,7 +1188,7 @@
                 <a:srgbClr val="008000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>≤</a:t>
+            <a:t>≥</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1205,35 +1197,35 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>26670</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5715</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>26670</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>5715</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>53341</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="204" name="OpenSolver7">
+        <xdr:cNvPr id="208" name="OpenSolver7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B8FB9D5-E0BF-41A3-956F-AEFA91155ACD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9AB481D-4D2A-4A74-ACA0-0464A10A216C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="202" idx="2"/>
-          <a:endCxn id="203" idx="0"/>
+          <a:stCxn id="206" idx="3"/>
+          <a:endCxn id="207" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6800850" y="15819120"/>
-          <a:ext cx="0" cy="365760"/>
+        <a:xfrm flipV="1">
+          <a:off x="4253865" y="14996160"/>
+          <a:ext cx="6324600" cy="1278256"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1266,23 +1258,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>453390</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>55880</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>455295</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>13970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>217170</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>169545</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>86995</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="205" name="OpenSolver8">
+        <xdr:cNvPr id="209" name="OpenSolver8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3C8F300-2365-45B6-97D4-3D8A4364CB0E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33EBEE71-4D36-4C91-AE97-D320DD489BF1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1290,7 +1282,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6610350" y="15875000"/>
+          <a:off x="7227570" y="15511145"/>
           <a:ext cx="381000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1651,22 +1643,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BFCD0C4-D6F5-4935-93E7-183ED66485B0}">
-  <dimension ref="A1:AE99"/>
+  <dimension ref="A1:AE90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P95" sqref="P95"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C49" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P51" sqref="P51:P54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
     <col min="10" max="11" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" customWidth="1"/>
+    <col min="16" max="16" width="11.5546875" customWidth="1"/>
     <col min="17" max="17" width="25.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.88671875" customWidth="1"/>
     <col min="24" max="24" width="8.88671875" customWidth="1"/>
@@ -2394,34 +2387,34 @@
       <c r="D20" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="86">
+      <c r="E20" s="78">
         <v>91524.65</v>
       </c>
-      <c r="F20" s="87">
+      <c r="F20" s="79">
         <v>255769.41</v>
       </c>
-      <c r="G20" s="87">
+      <c r="G20" s="79">
         <v>64363.94</v>
       </c>
-      <c r="H20" s="87">
+      <c r="H20" s="79">
         <v>2131.87</v>
       </c>
-      <c r="I20" s="88">
-        <v>0</v>
-      </c>
-      <c r="J20" s="88">
-        <v>0</v>
-      </c>
-      <c r="K20" s="88">
-        <v>0</v>
-      </c>
-      <c r="L20" s="88">
-        <v>0</v>
-      </c>
-      <c r="M20" s="88">
-        <v>0</v>
-      </c>
-      <c r="N20" s="89">
+      <c r="I20" s="80">
+        <v>0</v>
+      </c>
+      <c r="J20" s="80">
+        <v>0</v>
+      </c>
+      <c r="K20" s="80">
+        <v>0</v>
+      </c>
+      <c r="L20" s="80">
+        <v>0</v>
+      </c>
+      <c r="M20" s="80">
+        <v>0</v>
+      </c>
+      <c r="N20" s="81">
         <v>0</v>
       </c>
     </row>
@@ -2633,7 +2626,7 @@
         <f t="array" ref="R28:R37">MMULT(MINVERSE(_xlfn.MUNIT(10)-E28:N37),P28:P37)</f>
         <v>284820.45999999787</v>
       </c>
-      <c r="T28" s="95">
+      <c r="T28" s="87">
         <f>SUM(U28:Y28)</f>
         <v>1.0014327579401714</v>
       </c>
@@ -2697,7 +2690,7 @@
       <c r="R29" s="9">
         <v>973020.59999999811</v>
       </c>
-      <c r="T29" s="95">
+      <c r="T29" s="87">
         <f t="shared" ref="T29:T37" si="2">SUM(U29:Y29)</f>
         <v>1.0018296668824036</v>
       </c>
@@ -2760,7 +2753,7 @@
       <c r="R30" s="9">
         <v>2159997.7099999981</v>
       </c>
-      <c r="T30" s="95">
+      <c r="T30" s="87">
         <f>SUM(U30:Y30)</f>
         <v>1.0064020915194909</v>
       </c>
@@ -2823,7 +2816,7 @@
       <c r="R31" s="9">
         <v>84879.0799999999</v>
       </c>
-      <c r="T31" s="95">
+      <c r="T31" s="87">
         <f t="shared" si="2"/>
         <v>1.0027867254259681</v>
       </c>
@@ -2886,7 +2879,7 @@
       <c r="R32" s="22">
         <v>67274.930000000037</v>
       </c>
-      <c r="T32" s="96">
+      <c r="T32" s="88">
         <f t="shared" si="2"/>
         <v>1.0013910195243829</v>
       </c>
@@ -2949,7 +2942,7 @@
       <c r="R33" s="22">
         <v>913723.6100000001</v>
       </c>
-      <c r="T33" s="96">
+      <c r="T33" s="88">
         <f t="shared" si="2"/>
         <v>1.0024680208373091</v>
       </c>
@@ -3012,7 +3005,7 @@
       <c r="R34" s="22">
         <v>1648676.1800000004</v>
       </c>
-      <c r="T34" s="96">
+      <c r="T34" s="88">
         <f t="shared" si="2"/>
         <v>1.0019770740009657</v>
       </c>
@@ -3075,7 +3068,7 @@
       <c r="R35" s="22">
         <v>89574.700000000012</v>
       </c>
-      <c r="T35" s="96">
+      <c r="T35" s="88">
         <f t="shared" si="2"/>
         <v>1.0029054673635103</v>
       </c>
@@ -3138,7 +3131,7 @@
       <c r="R36" s="22">
         <v>199654.28000000006</v>
       </c>
-      <c r="T36" s="96">
+      <c r="T36" s="88">
         <f t="shared" si="2"/>
         <v>1.0032633018555592</v>
       </c>
@@ -3201,7 +3194,7 @@
       <c r="R37" s="22">
         <v>179240.77999999904</v>
       </c>
-      <c r="T37" s="96">
+      <c r="T37" s="88">
         <f t="shared" si="2"/>
         <v>1.0028838696389017</v>
       </c>
@@ -3381,75 +3374,75 @@
       <c r="D43" t="s">
         <v>22</v>
       </c>
-      <c r="E43" s="92">
+      <c r="E43" s="84">
         <v>0.32134155671260656</v>
       </c>
-      <c r="F43" s="93">
+      <c r="F43" s="85">
         <v>0.26286124877520634</v>
       </c>
-      <c r="G43" s="93">
+      <c r="G43" s="85">
         <v>2.9798151961929663E-2</v>
       </c>
-      <c r="H43" s="93">
+      <c r="H43" s="85">
         <v>2.51165540437055E-2</v>
       </c>
-      <c r="I43" s="93">
-        <v>0</v>
-      </c>
-      <c r="J43" s="93">
-        <v>0</v>
-      </c>
-      <c r="K43" s="93">
-        <v>0</v>
-      </c>
-      <c r="L43" s="93">
-        <v>0</v>
-      </c>
-      <c r="M43" s="93">
-        <v>0</v>
-      </c>
-      <c r="N43" s="94">
+      <c r="I43" s="85">
+        <v>0</v>
+      </c>
+      <c r="J43" s="85">
+        <v>0</v>
+      </c>
+      <c r="K43" s="85">
+        <v>0</v>
+      </c>
+      <c r="L43" s="85">
+        <v>0</v>
+      </c>
+      <c r="M43" s="85">
+        <v>0</v>
+      </c>
+      <c r="N43" s="86">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:25" x14ac:dyDescent="0.3">
-      <c r="E45" s="90">
+      <c r="E45" s="82">
         <f t="shared" ref="E45:N45" si="3">SUM(E28:E43)</f>
         <v>0.99999992978033303</v>
       </c>
-      <c r="F45" s="90">
+      <c r="F45" s="82">
         <f t="shared" si="3"/>
         <v>1.000022805272573</v>
       </c>
-      <c r="G45" s="90">
+      <c r="G45" s="82">
         <f t="shared" si="3"/>
         <v>1.0042566063646436</v>
       </c>
-      <c r="H45" s="90">
+      <c r="H45" s="82">
         <f t="shared" si="3"/>
         <v>1.0000008247026251</v>
       </c>
-      <c r="I45" s="91">
+      <c r="I45" s="83">
         <f t="shared" si="3"/>
         <v>0.99999881084974596</v>
       </c>
-      <c r="J45" s="91">
+      <c r="J45" s="83">
         <f t="shared" si="3"/>
         <v>1.0000001094422819</v>
       </c>
-      <c r="K45" s="91">
+      <c r="K45" s="83">
         <f t="shared" si="3"/>
         <v>1.000000103113031</v>
       </c>
-      <c r="L45" s="91">
+      <c r="L45" s="83">
         <f t="shared" si="3"/>
         <v>1.0000001116386645</v>
       </c>
-      <c r="M45" s="91">
+      <c r="M45" s="83">
         <f t="shared" si="3"/>
         <v>1.0000001001731589</v>
       </c>
-      <c r="N45" s="91">
+      <c r="N45" s="83">
         <f t="shared" si="3"/>
         <v>1.0000002231635066</v>
       </c>
@@ -3593,64 +3586,64 @@
       <c r="D51" t="s">
         <v>5</v>
       </c>
-      <c r="E51" s="97">
+      <c r="E51" s="89">
         <f t="shared" ref="E51:N51" si="4">E28</f>
         <v>0</v>
       </c>
-      <c r="F51" s="98">
+      <c r="F51" s="90">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G51" s="98">
+      <c r="G51" s="90">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H51" s="98">
+      <c r="H51" s="90">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I51" s="99">
+      <c r="I51" s="91">
         <f t="shared" si="4"/>
         <v>0.17504633598280817</v>
       </c>
-      <c r="J51" s="99">
+      <c r="J51" s="91">
         <f t="shared" si="4"/>
         <v>0.11741920513578388</v>
       </c>
-      <c r="K51" s="99">
+      <c r="K51" s="91">
         <f t="shared" si="4"/>
         <v>1.8225125324489132E-2</v>
       </c>
-      <c r="L51" s="99">
+      <c r="L51" s="91">
         <f t="shared" si="4"/>
         <v>6.060014713976155E-2</v>
       </c>
-      <c r="M51" s="99">
+      <c r="M51" s="91">
         <f t="shared" si="4"/>
         <v>5.1704376184672834E-3</v>
       </c>
-      <c r="N51" s="100">
+      <c r="N51" s="92">
         <f t="shared" si="4"/>
         <v>8.7173242606956355E-3</v>
       </c>
-      <c r="P51" s="82">
-        <v>6.7078476213232582E-2</v>
-      </c>
-      <c r="Q51" s="83"/>
+      <c r="P51" s="74">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q51" s="75"/>
       <c r="R51" s="9">
-        <v>569640.92000000004</v>
-      </c>
-      <c r="T51" s="84">
+        <v>349091.46</v>
+      </c>
+      <c r="T51" s="76">
         <f t="shared" ref="T51:T60" si="5">$R$64*P51</f>
-        <v>255370.32133064096</v>
-      </c>
-      <c r="V51" s="84">
+        <v>163879.48686279592</v>
+      </c>
+      <c r="V51" s="76">
         <f t="array" ref="V51:V60">MMULT(_xlfn.MUNIT(10)-E28:N37,R51:R60)</f>
-        <v>255370.32161938128</v>
-      </c>
-      <c r="X51" s="84">
+        <v>163879.4872453945</v>
+      </c>
+      <c r="X51" s="76">
         <f>SUM(E70:N70)+T51-R51</f>
-        <v>-2.88740498945117E-4</v>
+        <v>-3.8259854773059487E-4</v>
       </c>
       <c r="Z51" s="55">
         <f>SUM(AA51:AE51)</f>
@@ -3680,63 +3673,63 @@
       <c r="D52" t="s">
         <v>32</v>
       </c>
-      <c r="E52" s="101">
+      <c r="E52" s="93">
         <f t="shared" ref="E52:N52" si="6">E29</f>
         <v>0</v>
       </c>
-      <c r="F52" s="102">
+      <c r="F52" s="94">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G52" s="102">
+      <c r="G52" s="94">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="H52" s="102">
+      <c r="H52" s="94">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I52" s="103">
+      <c r="I52" s="95">
         <f t="shared" si="6"/>
         <v>0.1053665904966382</v>
       </c>
-      <c r="J52" s="103">
+      <c r="J52" s="95">
         <f t="shared" si="6"/>
         <v>0.35854581890468934</v>
       </c>
-      <c r="K52" s="103">
+      <c r="K52" s="95">
         <f t="shared" si="6"/>
         <v>4.7924329203324817E-2</v>
       </c>
-      <c r="L52" s="103">
+      <c r="L52" s="95">
         <f t="shared" si="6"/>
         <v>5.0928554603029641E-2</v>
       </c>
-      <c r="M52" s="103">
+      <c r="M52" s="95">
         <f t="shared" si="6"/>
         <v>0.17302674402972981</v>
       </c>
-      <c r="N52" s="104">
+      <c r="N52" s="96">
         <f t="shared" si="6"/>
         <v>0.11667383951353101</v>
       </c>
-      <c r="P52" s="82">
-        <v>0.26229757433112977</v>
-      </c>
-      <c r="Q52" s="83"/>
+      <c r="P52" s="74">
+        <v>0.22</v>
+      </c>
+      <c r="Q52" s="75"/>
       <c r="R52" s="9">
-        <v>1946041.2</v>
-      </c>
-      <c r="T52" s="84">
+        <v>1073655.6000000001</v>
+      </c>
+      <c r="T52" s="76">
         <f t="shared" si="5"/>
-        <v>998576.88520322321</v>
-      </c>
-      <c r="V52" s="84">
-        <v>998576.88525394478</v>
-      </c>
-      <c r="X52" s="84">
+        <v>515049.81585450139</v>
+      </c>
+      <c r="V52" s="76">
+        <v>515049.85246208264</v>
+      </c>
+      <c r="X52" s="76">
         <f t="shared" ref="X52:X60" si="7">SUM(E71:N71)+T52-R52</f>
-        <v>-5.0721690058708191E-5</v>
+        <v>-3.6607581423595548E-2</v>
       </c>
       <c r="Z52" s="55">
         <f t="shared" ref="Z52:Z60" si="8">SUM(AA52:AE52)</f>
@@ -3765,63 +3758,63 @@
       <c r="D53" t="s">
         <v>6</v>
       </c>
-      <c r="E53" s="101">
+      <c r="E53" s="93">
         <f t="shared" ref="E53:N53" si="9">E30</f>
         <v>0</v>
       </c>
-      <c r="F53" s="102">
+      <c r="F53" s="94">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G53" s="102">
+      <c r="G53" s="94">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="H53" s="102">
+      <c r="H53" s="94">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="I53" s="103">
+      <c r="I53" s="95">
         <f t="shared" si="9"/>
         <v>0.14037621443827589</v>
       </c>
-      <c r="J53" s="103">
+      <c r="J53" s="95">
         <f t="shared" si="9"/>
         <v>0.24880032376530031</v>
       </c>
-      <c r="K53" s="103">
+      <c r="K53" s="95">
         <f t="shared" si="9"/>
         <v>0.28668865101211022</v>
       </c>
-      <c r="L53" s="103">
+      <c r="L53" s="95">
         <f t="shared" si="9"/>
         <v>0.26061164592234076</v>
       </c>
-      <c r="M53" s="103">
+      <c r="M53" s="95">
         <f t="shared" si="9"/>
         <v>0.45838045645703118</v>
       </c>
-      <c r="N53" s="104">
+      <c r="N53" s="96">
         <f t="shared" si="9"/>
         <v>0.41069945131906038</v>
       </c>
-      <c r="P53" s="82">
-        <v>0.66302802878641021</v>
-      </c>
-      <c r="Q53" s="83"/>
+      <c r="P53" s="74">
+        <v>0.7</v>
+      </c>
+      <c r="Q53" s="75"/>
       <c r="R53" s="9">
-        <v>4319995.4000000004</v>
-      </c>
-      <c r="T53" s="84">
+        <v>2750841.8</v>
+      </c>
+      <c r="T53" s="76">
         <f t="shared" si="5"/>
-        <v>2524173.0331525588</v>
-      </c>
-      <c r="V53" s="84">
-        <v>2524172.9935084651</v>
-      </c>
-      <c r="X53" s="84">
+        <v>1638794.8686279589</v>
+      </c>
+      <c r="V53" s="76">
+        <v>1638794.8376030573</v>
+      </c>
+      <c r="X53" s="76">
         <f t="shared" si="7"/>
-        <v>3.9644094184041023E-2</v>
+        <v>3.1024901196360588E-2</v>
       </c>
       <c r="Z53" s="55">
         <f t="shared" si="8"/>
@@ -3850,63 +3843,63 @@
       <c r="D54" t="s">
         <v>33</v>
       </c>
-      <c r="E54" s="101">
+      <c r="E54" s="93">
         <f t="shared" ref="E54:N54" si="10">E31</f>
         <v>0</v>
       </c>
-      <c r="F54" s="102">
+      <c r="F54" s="94">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G54" s="102">
+      <c r="G54" s="94">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="H54" s="102">
+      <c r="H54" s="94">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="I54" s="103">
+      <c r="I54" s="95">
         <f t="shared" si="10"/>
         <v>1.7914399910932646E-2</v>
       </c>
-      <c r="J54" s="103">
+      <c r="J54" s="95">
         <f t="shared" si="10"/>
         <v>1.8235109411258398E-2</v>
       </c>
-      <c r="K54" s="103">
+      <c r="K54" s="95">
         <f t="shared" si="10"/>
         <v>9.9637213173055603E-3</v>
       </c>
-      <c r="L54" s="103">
+      <c r="L54" s="95">
         <f t="shared" si="10"/>
         <v>0.37925820572103502</v>
       </c>
-      <c r="M54" s="103">
+      <c r="M54" s="95">
         <f t="shared" si="10"/>
         <v>1.6574150075821068E-3</v>
       </c>
-      <c r="N54" s="104">
+      <c r="N54" s="96">
         <f t="shared" si="10"/>
         <v>1.017212712419579E-2</v>
       </c>
-      <c r="P54" s="82">
-        <v>7.5959206692274442E-3</v>
-      </c>
-      <c r="Q54" s="83"/>
+      <c r="P54" s="74">
+        <v>0.01</v>
+      </c>
+      <c r="Q54" s="75"/>
       <c r="R54" s="9">
-        <v>169758.16</v>
-      </c>
-      <c r="T54" s="84">
+        <v>112162.11</v>
+      </c>
+      <c r="T54" s="76">
         <f t="shared" si="5"/>
-        <v>28917.960150681098</v>
-      </c>
-      <c r="V54" s="84">
-        <v>28917.959966153525</v>
-      </c>
-      <c r="X54" s="84">
+        <v>23411.3552661137</v>
+      </c>
+      <c r="V54" s="76">
+        <v>23411.355371682163</v>
+      </c>
+      <c r="X54" s="76">
         <f t="shared" si="7"/>
-        <v>1.8452756921760738E-4</v>
+        <v>-1.0556845518294722E-4</v>
       </c>
       <c r="Z54" s="55">
         <f t="shared" si="8"/>
@@ -3935,63 +3928,63 @@
       <c r="D55" t="s">
         <v>7</v>
       </c>
-      <c r="E55" s="105">
+      <c r="E55" s="97">
         <f t="shared" ref="E55:N55" si="11">E32</f>
         <v>0.21743097388439181</v>
       </c>
-      <c r="F55" s="106">
+      <c r="F55" s="98">
         <f t="shared" si="11"/>
         <v>5.6537343608141619E-4</v>
       </c>
-      <c r="G55" s="106">
+      <c r="G55" s="98">
         <f t="shared" si="11"/>
         <v>1.5376358894380513E-3</v>
       </c>
-      <c r="H55" s="106">
+      <c r="H55" s="98">
         <f t="shared" si="11"/>
         <v>1.7374481438771506E-2</v>
       </c>
-      <c r="I55" s="102">
+      <c r="I55" s="94">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="J55" s="102">
+      <c r="J55" s="94">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K55" s="102">
+      <c r="K55" s="94">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="L55" s="102">
+      <c r="L55" s="94">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="M55" s="102">
+      <c r="M55" s="94">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="N55" s="107">
+      <c r="N55" s="99">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P55" s="21">
         <v>0</v>
       </c>
-      <c r="Q55" s="83"/>
+      <c r="Q55" s="75"/>
       <c r="R55" s="22">
-        <v>134549.85999999999</v>
-      </c>
-      <c r="T55" s="85">
+        <v>82688.865000000005</v>
+      </c>
+      <c r="T55" s="77">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V55" s="85">
-        <v>3.0751776648685336E-5</v>
-      </c>
-      <c r="X55" s="85">
+      <c r="V55" s="77">
+        <v>9.4556092517450452E-4</v>
+      </c>
+      <c r="X55" s="77">
         <f t="shared" si="7"/>
-        <v>-3.0751776648685336E-5</v>
+        <v>-9.4556092517450452E-4</v>
       </c>
       <c r="Z55" s="58">
         <f t="shared" si="8"/>
@@ -4020,63 +4013,63 @@
       <c r="D56" t="s">
         <v>34</v>
       </c>
-      <c r="E56" s="105">
+      <c r="E56" s="97">
         <f t="shared" ref="E56:N56" si="12">E33</f>
         <v>0.44390740047256771</v>
       </c>
-      <c r="F56" s="106">
+      <c r="F56" s="98">
         <f t="shared" si="12"/>
         <v>0.71162752361049852</v>
       </c>
-      <c r="G56" s="106">
+      <c r="G56" s="98">
         <f t="shared" si="12"/>
         <v>4.3108277184238361E-2</v>
       </c>
-      <c r="H56" s="106">
+      <c r="H56" s="98">
         <f t="shared" si="12"/>
         <v>2.0590232599127987E-2</v>
       </c>
-      <c r="I56" s="102">
+      <c r="I56" s="94">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="J56" s="102">
+      <c r="J56" s="94">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="K56" s="102">
+      <c r="K56" s="94">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="L56" s="102">
+      <c r="L56" s="94">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="M56" s="102">
+      <c r="M56" s="94">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="N56" s="107">
+      <c r="N56" s="99">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="P56" s="21">
         <v>0</v>
       </c>
-      <c r="Q56" s="83"/>
+      <c r="Q56" s="75"/>
       <c r="R56" s="22">
-        <v>1827447.2</v>
-      </c>
-      <c r="T56" s="85">
+        <v>1039900.6</v>
+      </c>
+      <c r="T56" s="77">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V56" s="85">
-        <v>-1.9137839321047068E-2</v>
-      </c>
-      <c r="X56" s="85">
+      <c r="V56" s="77">
+        <v>-5.3112415480427444E-2</v>
+      </c>
+      <c r="X56" s="77">
         <f t="shared" si="7"/>
-        <v>1.9137839321047068E-2</v>
+        <v>5.3112415480427444E-2</v>
       </c>
       <c r="Z56" s="58">
         <f t="shared" si="8"/>
@@ -4105,63 +4098,63 @@
       <c r="D57" t="s">
         <v>35</v>
       </c>
-      <c r="E57" s="105">
+      <c r="E57" s="97">
         <f t="shared" ref="E57:N57" si="13">E34</f>
         <v>1.6758171094871609E-2</v>
       </c>
-      <c r="F57" s="106">
+      <c r="F57" s="98">
         <f t="shared" si="13"/>
         <v>2.4641914056084787E-2</v>
       </c>
-      <c r="G57" s="106">
+      <c r="G57" s="98">
         <f t="shared" si="13"/>
         <v>0.74947286402447244</v>
       </c>
-      <c r="H57" s="106">
+      <c r="H57" s="98">
         <f t="shared" si="13"/>
         <v>1.2563166330266554E-2</v>
       </c>
-      <c r="I57" s="102">
+      <c r="I57" s="94">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="J57" s="102">
+      <c r="J57" s="94">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="K57" s="102">
+      <c r="K57" s="94">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="L57" s="102">
+      <c r="L57" s="94">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="M57" s="102">
+      <c r="M57" s="94">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="N57" s="107">
+      <c r="N57" s="99">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="P57" s="21">
         <v>0</v>
       </c>
-      <c r="Q57" s="83"/>
+      <c r="Q57" s="75"/>
       <c r="R57" s="22">
-        <v>3297352.4</v>
-      </c>
-      <c r="T57" s="85">
+        <v>2095397.5</v>
+      </c>
+      <c r="T57" s="77">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V57" s="85">
-        <v>5.4989452939480543E-2</v>
-      </c>
-      <c r="X57" s="85">
+      <c r="V57" s="77">
+        <v>4.2996408650651574E-2</v>
+      </c>
+      <c r="X57" s="77">
         <f t="shared" si="7"/>
-        <v>-5.4989452939480543E-2</v>
+        <v>-4.2996408650651574E-2</v>
       </c>
       <c r="Z57" s="58">
         <f t="shared" si="8"/>
@@ -4190,63 +4183,63 @@
       <c r="D58" t="s">
         <v>36</v>
       </c>
-      <c r="E58" s="105">
+      <c r="E58" s="97">
         <f t="shared" ref="E58:N58" si="14">E35</f>
         <v>4.2956885892256796E-4</v>
       </c>
-      <c r="F58" s="106">
+      <c r="F58" s="98">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="G58" s="106">
+      <c r="G58" s="98">
         <f t="shared" si="14"/>
         <v>5.1412971173937089E-3</v>
       </c>
-      <c r="H58" s="106">
+      <c r="H58" s="98">
         <f t="shared" si="14"/>
         <v>0.92304440623060591</v>
       </c>
-      <c r="I58" s="102">
+      <c r="I58" s="94">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="J58" s="102">
+      <c r="J58" s="94">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="K58" s="102">
+      <c r="K58" s="94">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="L58" s="102">
+      <c r="L58" s="94">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="M58" s="102">
+      <c r="M58" s="94">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="N58" s="107">
+      <c r="N58" s="99">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="P58" s="21">
         <v>0</v>
       </c>
-      <c r="Q58" s="83"/>
+      <c r="Q58" s="75"/>
       <c r="R58" s="22">
-        <v>179149.4</v>
-      </c>
-      <c r="T58" s="85">
+        <v>117823.46</v>
+      </c>
+      <c r="T58" s="77">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V58" s="85">
-        <v>1.0282569564878941E-4</v>
-      </c>
-      <c r="X58" s="85">
+      <c r="V58" s="77">
+        <v>-2.0633998356061056E-3</v>
+      </c>
+      <c r="X58" s="77">
         <f t="shared" si="7"/>
-        <v>-1.0282569564878941E-4</v>
+        <v>2.0633998356061056E-3</v>
       </c>
       <c r="Z58" s="58">
         <f t="shared" si="8"/>
@@ -4275,63 +4268,63 @@
       <c r="D59" t="s">
         <v>37</v>
       </c>
-      <c r="E59" s="105">
+      <c r="E59" s="97">
         <f t="shared" ref="E59:N59" si="15">E36</f>
         <v>1.13474994036595E-4</v>
       </c>
-      <c r="F59" s="106">
+      <c r="F59" s="98">
         <f t="shared" si="15"/>
         <v>2.699531746809878E-4</v>
       </c>
-      <c r="G59" s="106">
+      <c r="G59" s="98">
         <f t="shared" si="15"/>
         <v>9.2252769101315496E-2</v>
       </c>
-      <c r="H59" s="106">
+      <c r="H59" s="98">
         <f t="shared" si="15"/>
         <v>1.1018027056843701E-3</v>
       </c>
-      <c r="I59" s="102">
+      <c r="I59" s="94">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="J59" s="102">
+      <c r="J59" s="94">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="K59" s="102">
+      <c r="K59" s="94">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="L59" s="102">
+      <c r="L59" s="94">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="M59" s="102">
+      <c r="M59" s="94">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="N59" s="107">
+      <c r="N59" s="99">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="P59" s="21">
         <v>0</v>
       </c>
-      <c r="Q59" s="83"/>
+      <c r="Q59" s="75"/>
       <c r="R59" s="22">
-        <v>399308.56</v>
-      </c>
-      <c r="T59" s="85">
+        <v>254225.81</v>
+      </c>
+      <c r="T59" s="77">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V59" s="85">
-        <v>1.845054910518229E-3</v>
-      </c>
-      <c r="X59" s="85">
+      <c r="V59" s="77">
+        <v>6.185003905557096E-3</v>
+      </c>
+      <c r="X59" s="77">
         <f t="shared" si="7"/>
-        <v>-1.845054910518229E-3</v>
+        <v>-6.185003905557096E-3</v>
       </c>
       <c r="Z59" s="58">
         <f t="shared" si="8"/>
@@ -4360,63 +4353,63 @@
       <c r="D60" t="s">
         <v>38</v>
       </c>
-      <c r="E60" s="108">
+      <c r="E60" s="100">
         <f t="shared" ref="E60:N60" si="16">E37</f>
         <v>1.8783762936131907E-5</v>
       </c>
-      <c r="F60" s="109">
+      <c r="F60" s="101">
         <f t="shared" si="16"/>
         <v>5.6792220020830102E-5</v>
       </c>
-      <c r="G60" s="109">
+      <c r="G60" s="101">
         <f t="shared" si="16"/>
         <v>8.2945611085855825E-2</v>
       </c>
-      <c r="H60" s="109">
+      <c r="H60" s="101">
         <f t="shared" si="16"/>
         <v>2.1018135446331443E-4</v>
       </c>
-      <c r="I60" s="110">
+      <c r="I60" s="102">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="J60" s="110">
+      <c r="J60" s="102">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="K60" s="110">
+      <c r="K60" s="102">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="L60" s="110">
+      <c r="L60" s="102">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="M60" s="110">
+      <c r="M60" s="102">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="N60" s="111">
+      <c r="N60" s="103">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P60" s="21">
         <v>0</v>
       </c>
-      <c r="Q60" s="83"/>
+      <c r="Q60" s="75"/>
       <c r="R60" s="22">
-        <v>358481.56</v>
-      </c>
-      <c r="T60" s="85">
+        <v>228261.36</v>
+      </c>
+      <c r="T60" s="77">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="V60" s="85">
-        <v>1.6589138540439308E-3</v>
-      </c>
-      <c r="X60" s="85">
+      <c r="V60" s="77">
+        <v>-1.0220042895525694E-3</v>
+      </c>
+      <c r="X60" s="77">
         <f t="shared" si="7"/>
-        <v>-1.6589138540439308E-3</v>
+        <v>1.0220042895525694E-3</v>
       </c>
       <c r="Z60" s="58">
         <f t="shared" si="8"/>
@@ -4581,12 +4574,12 @@
         <f>N41</f>
         <v>0.12365495173587242</v>
       </c>
-      <c r="Q64" s="83" t="s">
+      <c r="Q64" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="R64" s="83">
+      <c r="R64" s="75">
         <f>SUM(V51:V60)</f>
-        <v>3807038.199837104</v>
+        <v>2341135.52661137</v>
       </c>
     </row>
     <row r="65" spans="3:24" x14ac:dyDescent="0.3">
@@ -4644,43 +4637,43 @@
       <c r="D66" t="s">
         <v>22</v>
       </c>
-      <c r="E66" s="92">
+      <c r="E66" s="84">
         <f t="shared" ref="E66:N66" si="21">E43</f>
         <v>0.32134155671260656</v>
       </c>
-      <c r="F66" s="93">
+      <c r="F66" s="85">
         <f t="shared" si="21"/>
         <v>0.26286124877520634</v>
       </c>
-      <c r="G66" s="93">
+      <c r="G66" s="85">
         <f t="shared" si="21"/>
         <v>2.9798151961929663E-2</v>
       </c>
-      <c r="H66" s="93">
+      <c r="H66" s="85">
         <f t="shared" si="21"/>
         <v>2.51165540437055E-2</v>
       </c>
-      <c r="I66" s="93">
+      <c r="I66" s="85">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="J66" s="93">
+      <c r="J66" s="85">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="K66" s="93">
+      <c r="K66" s="85">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="L66" s="93">
+      <c r="L66" s="85">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="M66" s="93">
+      <c r="M66" s="85">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
-      <c r="N66" s="94">
+      <c r="N66" s="86">
         <f t="shared" si="21"/>
         <v>0</v>
       </c>
@@ -4760,10 +4753,10 @@
       <c r="Q69" t="s">
         <v>5</v>
       </c>
-      <c r="R69" s="132">
+      <c r="R69" s="121">
         <v>6.7078476213232582E-2</v>
       </c>
-      <c r="S69" s="132">
+      <c r="S69" s="121">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -4774,44 +4767,44 @@
       <c r="D70" t="s">
         <v>5</v>
       </c>
-      <c r="E70" s="113">
+      <c r="E70" s="105">
         <f t="array" ref="E70:N79">MMULT(E51:N60,_xlfn.MUNIT(10)*R51:R60)</f>
         <v>0</v>
       </c>
-      <c r="F70" s="114">
-        <v>0</v>
-      </c>
-      <c r="G70" s="114">
-        <v>0</v>
-      </c>
-      <c r="H70" s="114">
-        <v>0</v>
-      </c>
-      <c r="I70" s="115">
-        <v>23552.459999999799</v>
-      </c>
-      <c r="J70" s="115">
-        <v>214577.39765161386</v>
-      </c>
-      <c r="K70" s="115">
-        <v>60094.660729005016</v>
-      </c>
-      <c r="L70" s="115">
-        <v>10856.479999999998</v>
-      </c>
-      <c r="M70" s="115">
-        <v>2064.6000000000004</v>
-      </c>
-      <c r="N70" s="116">
-        <v>3125.0000000000182</v>
+      <c r="F70" s="106">
+        <v>0</v>
+      </c>
+      <c r="G70" s="106">
+        <v>0</v>
+      </c>
+      <c r="H70" s="106">
+        <v>0</v>
+      </c>
+      <c r="I70" s="107">
+        <v>14474.382844827067</v>
+      </c>
+      <c r="J70" s="107">
+        <v>122104.30187222474</v>
+      </c>
+      <c r="K70" s="107">
+        <v>38188.882042121215</v>
+      </c>
+      <c r="L70" s="107">
+        <v>7140.11901251581</v>
+      </c>
+      <c r="M70" s="107">
+        <v>1314.458691609316</v>
+      </c>
+      <c r="N70" s="108">
+        <v>1989.8282913073801</v>
       </c>
       <c r="Q70" t="s">
         <v>32</v>
       </c>
-      <c r="R70" s="132">
+      <c r="R70" s="121">
         <v>0.26229757433112977</v>
       </c>
-      <c r="S70" s="132">
+      <c r="S70" s="121">
         <v>0.22</v>
       </c>
       <c r="X70" s="73"/>
@@ -4823,43 +4816,43 @@
       <c r="D71" t="s">
         <v>32</v>
       </c>
-      <c r="E71" s="117">
-        <v>0</v>
-      </c>
-      <c r="F71" s="118">
-        <v>0</v>
-      </c>
-      <c r="G71" s="118">
-        <v>0</v>
-      </c>
-      <c r="H71" s="118">
-        <v>0</v>
-      </c>
-      <c r="I71" s="119">
-        <v>14177.06</v>
-      </c>
-      <c r="J71" s="119">
-        <v>655223.55282908154</v>
-      </c>
-      <c r="K71" s="119">
-        <v>158023.40191697318</v>
-      </c>
-      <c r="L71" s="119">
-        <v>9123.8199999999979</v>
-      </c>
-      <c r="M71" s="119">
-        <v>69091.060000000012</v>
-      </c>
-      <c r="N71" s="120">
-        <v>41825.420000000238</v>
+      <c r="E71" s="109">
+        <v>0</v>
+      </c>
+      <c r="F71" s="110">
+        <v>0</v>
+      </c>
+      <c r="G71" s="110">
+        <v>0</v>
+      </c>
+      <c r="H71" s="110">
+        <v>0</v>
+      </c>
+      <c r="I71" s="111">
+        <v>8712.6437770867997</v>
+      </c>
+      <c r="J71" s="111">
+        <v>372852.01220647775</v>
+      </c>
+      <c r="K71" s="111">
+        <v>100420.51960182382</v>
+      </c>
+      <c r="L71" s="111">
+        <v>6000.5785161278791</v>
+      </c>
+      <c r="M71" s="111">
+        <v>43987.864152620728</v>
+      </c>
+      <c r="N71" s="112">
+        <v>26632.129283780327</v>
       </c>
       <c r="Q71" t="s">
         <v>6</v>
       </c>
-      <c r="R71" s="132">
+      <c r="R71" s="121">
         <v>0.66302802878641021</v>
       </c>
-      <c r="S71" s="132">
+      <c r="S71" s="121">
         <v>0.7</v>
       </c>
       <c r="X71" s="73"/>
@@ -4871,43 +4864,43 @@
       <c r="D72" t="s">
         <v>6</v>
       </c>
-      <c r="E72" s="117">
-        <v>0</v>
-      </c>
-      <c r="F72" s="118">
-        <v>0</v>
-      </c>
-      <c r="G72" s="118">
-        <v>0</v>
-      </c>
-      <c r="H72" s="118">
-        <v>0</v>
-      </c>
-      <c r="I72" s="119">
-        <v>18887.599999999999</v>
-      </c>
-      <c r="J72" s="119">
-        <v>454669.45502399153</v>
-      </c>
-      <c r="K72" s="119">
-        <v>945313.51146754401</v>
-      </c>
-      <c r="L72" s="119">
-        <v>46688.419999999795</v>
-      </c>
-      <c r="M72" s="119">
-        <v>183035.23999999982</v>
-      </c>
-      <c r="N72" s="120">
-        <v>147228.18000000084</v>
+      <c r="E72" s="109">
+        <v>0</v>
+      </c>
+      <c r="F72" s="110">
+        <v>0</v>
+      </c>
+      <c r="G72" s="110">
+        <v>0</v>
+      </c>
+      <c r="H72" s="110">
+        <v>0</v>
+      </c>
+      <c r="I72" s="111">
+        <v>11607.549844897647</v>
+      </c>
+      <c r="J72" s="111">
+        <v>258727.60596373005</v>
+      </c>
+      <c r="K72" s="111">
+        <v>600726.68260914821</v>
+      </c>
+      <c r="L72" s="111">
+        <v>30706.165838865083</v>
+      </c>
+      <c r="M72" s="111">
+        <v>116532.14283095849</v>
+      </c>
+      <c r="N72" s="112">
+        <v>93746.815309342506</v>
       </c>
       <c r="Q72" t="s">
         <v>33</v>
       </c>
-      <c r="R72" s="132">
+      <c r="R72" s="121">
         <v>7.5959206692274442E-3</v>
       </c>
-      <c r="S72" s="132">
+      <c r="S72" s="121">
         <v>0.01</v>
       </c>
       <c r="X72" s="73"/>
@@ -4919,35 +4912,35 @@
       <c r="D73" t="s">
         <v>33</v>
       </c>
-      <c r="E73" s="117">
-        <v>0</v>
-      </c>
-      <c r="F73" s="118">
-        <v>0</v>
-      </c>
-      <c r="G73" s="118">
-        <v>0</v>
-      </c>
-      <c r="H73" s="118">
-        <v>0</v>
-      </c>
-      <c r="I73" s="119">
-        <v>2410.3799999999997</v>
-      </c>
-      <c r="J73" s="119">
-        <v>33323.699635297809</v>
-      </c>
-      <c r="K73" s="119">
-        <v>32853.900398548649</v>
-      </c>
-      <c r="L73" s="119">
-        <v>67943.87999999999</v>
-      </c>
-      <c r="M73" s="119">
-        <v>661.82000000000016</v>
-      </c>
-      <c r="N73" s="120">
-        <v>3646.5200000000204</v>
+      <c r="E73" s="109">
+        <v>0</v>
+      </c>
+      <c r="F73" s="110">
+        <v>0</v>
+      </c>
+      <c r="G73" s="110">
+        <v>0</v>
+      </c>
+      <c r="H73" s="110">
+        <v>0</v>
+      </c>
+      <c r="I73" s="111">
+        <v>1481.3213957911216</v>
+      </c>
+      <c r="J73" s="111">
+        <v>18962.701217833255</v>
+      </c>
+      <c r="K73" s="111">
+        <v>20877.956738978777</v>
+      </c>
+      <c r="L73" s="111">
+        <v>44685.514031444145</v>
+      </c>
+      <c r="M73" s="111">
+        <v>421.35767280871721</v>
+      </c>
+      <c r="N73" s="112">
+        <v>2321.9035714618199</v>
       </c>
       <c r="T73" s="68"/>
       <c r="X73" s="73"/>
@@ -4959,34 +4952,34 @@
       <c r="D74" t="s">
         <v>7</v>
       </c>
-      <c r="E74" s="121">
-        <v>123857.58000000093</v>
-      </c>
-      <c r="F74" s="122">
-        <v>1100.2400000000025</v>
-      </c>
-      <c r="G74" s="122">
-        <v>6642.579969247291</v>
-      </c>
-      <c r="H74" s="122">
-        <v>2949.4600000000037</v>
-      </c>
-      <c r="I74" s="118">
-        <v>0</v>
-      </c>
-      <c r="J74" s="118">
-        <v>0</v>
-      </c>
-      <c r="K74" s="118">
-        <v>0</v>
-      </c>
-      <c r="L74" s="118">
-        <v>0</v>
-      </c>
-      <c r="M74" s="118">
-        <v>0</v>
-      </c>
-      <c r="N74" s="123">
+      <c r="E74" s="113">
+        <v>75903.296122524218</v>
+      </c>
+      <c r="F74" s="114">
+        <v>607.01635574005456</v>
+      </c>
+      <c r="G74" s="114">
+        <v>4229.7930778463697</v>
+      </c>
+      <c r="H74" s="114">
+        <v>1948.758498328448</v>
+      </c>
+      <c r="I74" s="110">
+        <v>0</v>
+      </c>
+      <c r="J74" s="110">
+        <v>0</v>
+      </c>
+      <c r="K74" s="110">
+        <v>0</v>
+      </c>
+      <c r="L74" s="110">
+        <v>0</v>
+      </c>
+      <c r="M74" s="110">
+        <v>0</v>
+      </c>
+      <c r="N74" s="115">
         <v>0</v>
       </c>
       <c r="T74" s="68"/>
@@ -4999,34 +4992,34 @@
       <c r="D75" t="s">
         <v>34</v>
       </c>
-      <c r="E75" s="121">
-        <v>252867.82000000193</v>
-      </c>
-      <c r="F75" s="122">
-        <v>1384856.4800000028</v>
-      </c>
-      <c r="G75" s="122">
-        <v>186227.5591378347</v>
-      </c>
-      <c r="H75" s="122">
-        <v>3495.3599999999847</v>
-      </c>
-      <c r="I75" s="118">
-        <v>0</v>
-      </c>
-      <c r="J75" s="118">
-        <v>0</v>
-      </c>
-      <c r="K75" s="118">
-        <v>0</v>
-      </c>
-      <c r="L75" s="118">
-        <v>0</v>
-      </c>
-      <c r="M75" s="118">
-        <v>0</v>
-      </c>
-      <c r="N75" s="123">
+      <c r="E75" s="113">
+        <v>154964.28253577335</v>
+      </c>
+      <c r="F75" s="114">
+        <v>764042.87583854399</v>
+      </c>
+      <c r="G75" s="114">
+        <v>118584.05080438918</v>
+      </c>
+      <c r="H75" s="114">
+        <v>2309.4439337089793</v>
+      </c>
+      <c r="I75" s="110">
+        <v>0</v>
+      </c>
+      <c r="J75" s="110">
+        <v>0</v>
+      </c>
+      <c r="K75" s="110">
+        <v>0</v>
+      </c>
+      <c r="L75" s="110">
+        <v>0</v>
+      </c>
+      <c r="M75" s="110">
+        <v>0</v>
+      </c>
+      <c r="N75" s="115">
         <v>0</v>
       </c>
       <c r="T75" s="68"/>
@@ -5039,34 +5032,34 @@
       <c r="D76" t="s">
         <v>35</v>
       </c>
-      <c r="E76" s="121">
-        <v>9546.1400000000722</v>
-      </c>
-      <c r="F76" s="122">
-        <v>47954.180000000102</v>
-      </c>
-      <c r="G76" s="122">
-        <v>3237719.3250105465</v>
-      </c>
-      <c r="H76" s="122">
-        <v>2132.7000000000025</v>
-      </c>
-      <c r="I76" s="118">
-        <v>0</v>
-      </c>
-      <c r="J76" s="118">
-        <v>0</v>
-      </c>
-      <c r="K76" s="118">
-        <v>0</v>
-      </c>
-      <c r="L76" s="118">
-        <v>0</v>
-      </c>
-      <c r="M76" s="118">
-        <v>0</v>
-      </c>
-      <c r="N76" s="123">
+      <c r="E76" s="113">
+        <v>5850.1344144385293</v>
+      </c>
+      <c r="F76" s="114">
+        <v>26456.92902103415</v>
+      </c>
+      <c r="G76" s="114">
+        <v>2061681.282324235</v>
+      </c>
+      <c r="H76" s="114">
+        <v>1409.1112438836535</v>
+      </c>
+      <c r="I76" s="110">
+        <v>0</v>
+      </c>
+      <c r="J76" s="110">
+        <v>0</v>
+      </c>
+      <c r="K76" s="110">
+        <v>0</v>
+      </c>
+      <c r="L76" s="110">
+        <v>0</v>
+      </c>
+      <c r="M76" s="110">
+        <v>0</v>
+      </c>
+      <c r="N76" s="115">
         <v>0</v>
       </c>
     </row>
@@ -5077,34 +5070,34 @@
       <c r="D77" t="s">
         <v>36</v>
       </c>
-      <c r="E77" s="121">
-        <v>244.70000000000184</v>
-      </c>
-      <c r="F77" s="122">
-        <v>0</v>
-      </c>
-      <c r="G77" s="122">
-        <v>22210.379897174083</v>
-      </c>
-      <c r="H77" s="122">
-        <v>156694.32000000021</v>
-      </c>
-      <c r="I77" s="118">
-        <v>0</v>
-      </c>
-      <c r="J77" s="118">
-        <v>0</v>
-      </c>
-      <c r="K77" s="118">
-        <v>0</v>
-      </c>
-      <c r="L77" s="118">
-        <v>0</v>
-      </c>
-      <c r="M77" s="118">
-        <v>0</v>
-      </c>
-      <c r="N77" s="123">
+      <c r="E77" s="113">
+        <v>149.9588201318133</v>
+      </c>
+      <c r="F77" s="114">
+        <v>0</v>
+      </c>
+      <c r="G77" s="114">
+        <v>14142.895016746121</v>
+      </c>
+      <c r="H77" s="114">
+        <v>103530.6082265219</v>
+      </c>
+      <c r="I77" s="110">
+        <v>0</v>
+      </c>
+      <c r="J77" s="110">
+        <v>0</v>
+      </c>
+      <c r="K77" s="110">
+        <v>0</v>
+      </c>
+      <c r="L77" s="110">
+        <v>0</v>
+      </c>
+      <c r="M77" s="110">
+        <v>0</v>
+      </c>
+      <c r="N77" s="115">
         <v>0</v>
       </c>
     </row>
@@ -5115,34 +5108,34 @@
       <c r="D78" t="s">
         <v>37</v>
       </c>
-      <c r="E78" s="121">
-        <v>64.640000000000498</v>
-      </c>
-      <c r="F78" s="122">
-        <v>525.33999999999912</v>
-      </c>
-      <c r="G78" s="122">
-        <v>398531.53815494513</v>
-      </c>
-      <c r="H78" s="122">
-        <v>187.04000000000022</v>
-      </c>
-      <c r="I78" s="118">
-        <v>0</v>
-      </c>
-      <c r="J78" s="118">
-        <v>0</v>
-      </c>
-      <c r="K78" s="118">
-        <v>0</v>
-      </c>
-      <c r="L78" s="118">
-        <v>0</v>
-      </c>
-      <c r="M78" s="118">
-        <v>0</v>
-      </c>
-      <c r="N78" s="123">
+      <c r="E78" s="113">
+        <v>39.613151341726244</v>
+      </c>
+      <c r="F78" s="114">
+        <v>289.8367377340208</v>
+      </c>
+      <c r="G78" s="114">
+        <v>253772.77340964708</v>
+      </c>
+      <c r="H78" s="114">
+        <v>123.58051627326795</v>
+      </c>
+      <c r="I78" s="110">
+        <v>0</v>
+      </c>
+      <c r="J78" s="110">
+        <v>0</v>
+      </c>
+      <c r="K78" s="110">
+        <v>0</v>
+      </c>
+      <c r="L78" s="110">
+        <v>0</v>
+      </c>
+      <c r="M78" s="110">
+        <v>0</v>
+      </c>
+      <c r="N78" s="115">
         <v>0</v>
       </c>
     </row>
@@ -5153,46 +5146,43 @@
       <c r="D79" t="s">
         <v>38</v>
       </c>
-      <c r="E79" s="124">
-        <v>10.700000000000081</v>
-      </c>
-      <c r="F79" s="125">
-        <v>110.52000000000024</v>
-      </c>
-      <c r="G79" s="125">
-        <v>358324.65834108618</v>
-      </c>
-      <c r="H79" s="125">
-        <v>35.680000000000042</v>
-      </c>
-      <c r="I79" s="126">
-        <v>0</v>
-      </c>
-      <c r="J79" s="126">
-        <v>0</v>
-      </c>
-      <c r="K79" s="126">
-        <v>0</v>
-      </c>
-      <c r="L79" s="126">
-        <v>0</v>
-      </c>
-      <c r="M79" s="126">
-        <v>0</v>
-      </c>
-      <c r="N79" s="127">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="E79" s="116">
+        <v>6.557251227668174</v>
+      </c>
+      <c r="F79" s="117">
+        <v>60.975285061796363</v>
+      </c>
+      <c r="G79" s="117">
+        <v>228170.25410151557</v>
+      </c>
+      <c r="H79" s="117">
+        <v>23.574384199263264</v>
+      </c>
+      <c r="I79" s="118">
+        <v>0</v>
+      </c>
+      <c r="J79" s="118">
+        <v>0</v>
+      </c>
+      <c r="K79" s="118">
+        <v>0</v>
+      </c>
+      <c r="L79" s="118">
+        <v>0</v>
+      </c>
+      <c r="M79" s="118">
+        <v>0</v>
+      </c>
+      <c r="N79" s="119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C81" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="U81">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="82" spans="3:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C82" t="s">
         <v>19</v>
       </c>
@@ -5213,38 +5203,32 @@
         <v>0</v>
       </c>
       <c r="I82" s="69">
-        <v>19142.68</v>
+        <v>11764.311625877577</v>
       </c>
       <c r="J82" s="69">
-        <v>268535.95706108108</v>
+        <v>152809.1771239095</v>
       </c>
       <c r="K82" s="69">
-        <v>855329.8503759572</v>
+        <v>543543.9749033663</v>
       </c>
       <c r="L82" s="69">
-        <v>10742.399999999996</v>
+        <v>7065.0905707973325</v>
       </c>
       <c r="M82" s="69">
-        <v>60124.520000000004</v>
+        <v>38279.181387599609</v>
       </c>
       <c r="N82" s="70">
-        <v>64639.260000000366</v>
-      </c>
-      <c r="P82" s="112">
-        <f>SUM(I82:N85)/(10^6)</f>
-        <v>2.9978919803479367</v>
+        <v>41158.72904869551</v>
+      </c>
+      <c r="P82" s="123">
+        <f>SUM(I82:N85)</f>
+        <v>1873682.4787844762</v>
       </c>
       <c r="Q82" t="s">
         <v>43</v>
       </c>
-      <c r="U82" s="112">
-        <v>1.498945992743965</v>
-      </c>
-      <c r="V82" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="83" spans="3:22" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C83" t="s">
         <v>19</v>
       </c>
@@ -5267,22 +5251,22 @@
         <v>0</v>
       </c>
       <c r="J83" s="71">
-        <v>28438.319688764524</v>
+        <v>16182.697758566181</v>
       </c>
       <c r="K83" s="71">
-        <v>144095.82174801826</v>
+        <v>91569.837864840621</v>
       </c>
       <c r="L83" s="71">
         <v>0</v>
       </c>
       <c r="M83" s="71">
-        <v>7503.0000000000009</v>
+        <v>4776.8979769179014</v>
       </c>
       <c r="N83" s="72">
-        <v>15256.140000000087</v>
-      </c>
-    </row>
-    <row r="84" spans="3:22" x14ac:dyDescent="0.3">
+        <v>9714.2716762067757</v>
+      </c>
+    </row>
+    <row r="84" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C84" t="s">
         <v>19</v>
       </c>
@@ -5302,25 +5286,25 @@
         <v>0</v>
       </c>
       <c r="I84" s="71">
-        <v>30400.799999999996</v>
+        <v>18683.093740060376</v>
       </c>
       <c r="J84" s="71">
-        <v>119813.11868873762</v>
+        <v>68179.11566051784</v>
       </c>
       <c r="K84" s="71">
-        <v>213023.04258417079</v>
+        <v>135371.62448067882</v>
       </c>
       <c r="L84" s="71">
-        <v>28218.979999999996</v>
+        <v>18559.134785105613</v>
       </c>
       <c r="M84" s="71">
-        <v>16665.18</v>
+        <v>10610.137895104979</v>
       </c>
       <c r="N84" s="72">
-        <v>44328.020000000251</v>
-      </c>
-    </row>
-    <row r="85" spans="3:22" x14ac:dyDescent="0.3">
+        <v>28225.647453964597</v>
+      </c>
+    </row>
+    <row r="85" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C85" t="s">
         <v>19</v>
       </c>
@@ -5340,461 +5324,111 @@
         <v>0</v>
       </c>
       <c r="I85" s="71">
-        <v>25978.720000000001</v>
+        <v>15965.4634419746</v>
       </c>
       <c r="J85" s="71">
-        <v>52865.899421423514</v>
+        <v>30083.102005835222</v>
       </c>
       <c r="K85" s="71">
-        <v>888618.5507797827</v>
+        <v>564698.23782182939</v>
       </c>
       <c r="L85" s="71">
-        <v>5575.4399999999978</v>
+        <v>3666.8703987978738</v>
       </c>
       <c r="M85" s="71">
-        <v>60163.180000000008</v>
+        <v>38303.794858982743</v>
       </c>
       <c r="N85" s="72">
-        <v>38433.100000000217</v>
-      </c>
-    </row>
-    <row r="86" spans="3:22" x14ac:dyDescent="0.3">
+        <v>24472.086304846613</v>
+      </c>
+    </row>
+    <row r="86" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C86" t="s">
         <v>41</v>
       </c>
       <c r="D86" t="s">
         <v>22</v>
       </c>
-      <c r="E86" s="86">
-        <v>183049.30000000139</v>
-      </c>
-      <c r="F86" s="87">
-        <v>511538.82000000105</v>
-      </c>
-      <c r="G86" s="87">
-        <v>128727.87940403713</v>
-      </c>
-      <c r="H86" s="87">
-        <v>4263.7400000000052</v>
-      </c>
-      <c r="I86" s="87">
-        <v>0</v>
-      </c>
-      <c r="J86" s="87">
-        <v>0</v>
-      </c>
-      <c r="K86" s="87">
-        <v>0</v>
-      </c>
-      <c r="L86" s="87">
-        <v>0</v>
-      </c>
-      <c r="M86" s="87">
-        <v>0</v>
-      </c>
-      <c r="N86" s="131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="3:22" x14ac:dyDescent="0.3">
+      <c r="E86" s="78">
+        <v>112177.59319147663</v>
+      </c>
+      <c r="F86" s="79">
+        <v>282222.45177049347</v>
+      </c>
+      <c r="G86" s="79">
+        <v>81970.001979628127</v>
+      </c>
+      <c r="H86" s="79">
+        <v>2817.1256974710413</v>
+      </c>
+      <c r="I86" s="79">
+        <v>0</v>
+      </c>
+      <c r="J86" s="79">
+        <v>0</v>
+      </c>
+      <c r="K86" s="79">
+        <v>0</v>
+      </c>
+      <c r="L86" s="79">
+        <v>0</v>
+      </c>
+      <c r="M86" s="79">
+        <v>0</v>
+      </c>
+      <c r="N86" s="120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="I87" s="124">
+        <f>SUM(I$82:I$85)/SUM($I$82:$N$85)</f>
+        <v>2.4770936022213443E-2</v>
+      </c>
+      <c r="J87" s="124">
+        <f t="shared" ref="J87:N87" si="22">SUM(J$82:J$85)/SUM($I$82:$N$85)</f>
+        <v>0.14263574302205456</v>
+      </c>
+      <c r="K87" s="124">
+        <f t="shared" si="22"/>
+        <v>0.71259868744510857</v>
+      </c>
+      <c r="L87" s="124">
+        <f t="shared" si="22"/>
+        <v>1.5632902632308855E-2</v>
+      </c>
+      <c r="M87" s="124">
+        <f t="shared" si="22"/>
+        <v>4.9085164194025775E-2</v>
+      </c>
+      <c r="N87" s="124">
+        <f t="shared" si="22"/>
+        <v>5.5276566684288729E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C88" s="67" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="89" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C89" t="s">
-        <v>19</v>
-      </c>
-      <c r="D89" t="s">
-        <v>39</v>
-      </c>
-      <c r="E89" s="31">
-        <f t="array" ref="E89:N93">E16:N20*E95:N99</f>
-        <v>0</v>
-      </c>
-      <c r="F89" s="32">
-        <v>0</v>
-      </c>
-      <c r="G89" s="32">
-        <v>0</v>
-      </c>
-      <c r="H89" s="32">
-        <v>0</v>
-      </c>
-      <c r="I89" s="69">
-        <v>19142.68</v>
-      </c>
-      <c r="J89" s="69">
-        <v>268535.96000000002</v>
-      </c>
-      <c r="K89" s="69">
-        <v>855329.83999999799</v>
-      </c>
-      <c r="L89" s="69">
-        <v>10742.4</v>
-      </c>
-      <c r="M89" s="69">
-        <v>60124.52</v>
-      </c>
-      <c r="N89" s="70">
-        <v>64639.26</v>
-      </c>
-      <c r="P89" s="112">
+        <v>43</v>
+      </c>
+      <c r="D89">
+        <v>2015</v>
+      </c>
+      <c r="E89" s="123">
+        <f>1.25*1498945.98</f>
+        <v>1873682.4750000001</v>
+      </c>
+      <c r="P89" s="104">
         <f>SUM(I89:N92)/(10^6)</f>
-        <v>2.9978919599999978</v>
-      </c>
-      <c r="Q89" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="90" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C90" t="s">
-        <v>19</v>
-      </c>
-      <c r="D90" t="s">
-        <v>21</v>
-      </c>
-      <c r="E90" s="35">
-        <v>0</v>
-      </c>
-      <c r="F90" s="36">
-        <v>0</v>
-      </c>
-      <c r="G90" s="36">
-        <v>0</v>
-      </c>
-      <c r="H90" s="36">
-        <v>0</v>
-      </c>
-      <c r="I90" s="71">
-        <v>0</v>
-      </c>
-      <c r="J90" s="71">
-        <v>28438.32</v>
-      </c>
-      <c r="K90" s="71">
-        <v>144095.8199999998</v>
-      </c>
-      <c r="L90" s="71">
-        <v>0</v>
-      </c>
-      <c r="M90" s="71">
-        <v>7503</v>
-      </c>
-      <c r="N90" s="72">
-        <v>15256.14</v>
-      </c>
-      <c r="P90" s="134">
-        <f>(P82-U82)/U82</f>
-        <v>0.99999999657092831</v>
-      </c>
-    </row>
-    <row r="91" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C91" t="s">
-        <v>19</v>
-      </c>
-      <c r="D91" t="s">
-        <v>20</v>
-      </c>
-      <c r="E91" s="35">
-        <v>0</v>
-      </c>
-      <c r="F91" s="36">
-        <v>0</v>
-      </c>
-      <c r="G91" s="36">
-        <v>0</v>
-      </c>
-      <c r="H91" s="36">
-        <v>0</v>
-      </c>
-      <c r="I91" s="71">
-        <v>30400.799999999999</v>
-      </c>
-      <c r="J91" s="71">
-        <v>119813.11999999981</v>
-      </c>
-      <c r="K91" s="71">
-        <v>213023.04</v>
-      </c>
-      <c r="L91" s="71">
-        <v>28218.98</v>
-      </c>
-      <c r="M91" s="71">
-        <v>16665.18</v>
-      </c>
-      <c r="N91" s="72">
-        <v>44328.02</v>
-      </c>
-    </row>
-    <row r="92" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C92" t="s">
-        <v>19</v>
-      </c>
-      <c r="D92" t="s">
-        <v>40</v>
-      </c>
-      <c r="E92" s="35">
-        <v>0</v>
-      </c>
-      <c r="F92" s="36">
-        <v>0</v>
-      </c>
-      <c r="G92" s="36">
-        <v>0</v>
-      </c>
-      <c r="H92" s="36">
-        <v>0</v>
-      </c>
-      <c r="I92" s="71">
-        <v>25978.720000000001</v>
-      </c>
-      <c r="J92" s="71">
-        <v>52865.9</v>
-      </c>
-      <c r="K92" s="71">
-        <v>888618.54</v>
-      </c>
-      <c r="L92" s="71">
-        <v>5575.44</v>
-      </c>
-      <c r="M92" s="71">
-        <v>60163.18</v>
-      </c>
-      <c r="N92" s="72">
-        <v>38433.1</v>
-      </c>
-    </row>
-    <row r="93" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C93" t="s">
-        <v>41</v>
-      </c>
-      <c r="D93" t="s">
-        <v>22</v>
-      </c>
-      <c r="E93" s="86">
-        <v>183049.3</v>
-      </c>
-      <c r="F93" s="87">
-        <v>511538.82</v>
-      </c>
-      <c r="G93" s="87">
-        <v>128727.88</v>
-      </c>
-      <c r="H93" s="87">
-        <v>4263.74</v>
-      </c>
-      <c r="I93" s="87">
-        <v>0</v>
-      </c>
-      <c r="J93" s="87">
-        <v>0</v>
-      </c>
-      <c r="K93" s="87">
-        <v>0</v>
-      </c>
-      <c r="L93" s="87">
-        <v>0</v>
-      </c>
-      <c r="M93" s="87">
-        <v>0</v>
-      </c>
-      <c r="N93" s="131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C95" t="s">
-        <v>19</v>
-      </c>
-      <c r="D95" t="s">
-        <v>39</v>
-      </c>
-      <c r="E95" s="74"/>
-      <c r="F95" s="75"/>
-      <c r="G95" s="75"/>
-      <c r="H95" s="75"/>
-      <c r="I95" s="76">
-        <f>$P$95</f>
-        <v>2</v>
-      </c>
-      <c r="J95" s="76">
-        <f t="shared" ref="J95:N98" si="22">$P$95</f>
-        <v>2</v>
-      </c>
-      <c r="K95" s="76">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="L95" s="76">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="M95" s="76">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="N95" s="77">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="P95" s="133">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96" spans="3:22" x14ac:dyDescent="0.3">
-      <c r="C96" t="s">
-        <v>19</v>
-      </c>
-      <c r="D96" t="s">
-        <v>21</v>
-      </c>
-      <c r="E96" s="78"/>
-      <c r="F96" s="79"/>
-      <c r="G96" s="79"/>
-      <c r="H96" s="79"/>
-      <c r="I96" s="80">
-        <f t="shared" ref="I96:I98" si="23">$P$95</f>
-        <v>2</v>
-      </c>
-      <c r="J96" s="80">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="K96" s="80">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="L96" s="80">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="M96" s="80">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="N96" s="81">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C97" t="s">
-        <v>19</v>
-      </c>
-      <c r="D97" t="s">
-        <v>20</v>
-      </c>
-      <c r="E97" s="78">
-        <v>0</v>
-      </c>
-      <c r="F97" s="79">
-        <v>0</v>
-      </c>
-      <c r="G97" s="79">
-        <v>0</v>
-      </c>
-      <c r="H97" s="79">
-        <v>0</v>
-      </c>
-      <c r="I97" s="80">
-        <f t="shared" si="23"/>
-        <v>2</v>
-      </c>
-      <c r="J97" s="80">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="K97" s="80">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="L97" s="80">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="M97" s="80">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="N97" s="81">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C98" t="s">
-        <v>19</v>
-      </c>
-      <c r="D98" t="s">
-        <v>40</v>
-      </c>
-      <c r="E98" s="78">
-        <v>0</v>
-      </c>
-      <c r="F98" s="79">
-        <v>0</v>
-      </c>
-      <c r="G98" s="79">
-        <v>0</v>
-      </c>
-      <c r="H98" s="79">
-        <v>0</v>
-      </c>
-      <c r="I98" s="80">
-        <f t="shared" si="23"/>
-        <v>2</v>
-      </c>
-      <c r="J98" s="80">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="K98" s="80">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="L98" s="80">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="M98" s="80">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-      <c r="N98" s="81">
-        <f t="shared" si="22"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C99" t="s">
-        <v>41</v>
-      </c>
-      <c r="D99" t="s">
-        <v>22</v>
-      </c>
-      <c r="E99" s="128">
-        <f t="shared" ref="E99:H99" si="24">$P$95</f>
-        <v>2</v>
-      </c>
-      <c r="F99" s="129">
-        <f t="shared" si="24"/>
-        <v>2</v>
-      </c>
-      <c r="G99" s="129">
-        <f t="shared" si="24"/>
-        <v>2</v>
-      </c>
-      <c r="H99" s="129">
-        <f t="shared" si="24"/>
-        <v>2</v>
-      </c>
-      <c r="I99" s="129"/>
-      <c r="J99" s="129"/>
-      <c r="K99" s="129"/>
-      <c r="L99" s="129"/>
-      <c r="M99" s="129"/>
-      <c r="N99" s="130"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P90" s="122"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>